<commit_message>
#0 컨트롤러 DAO SearchDTO 생성
</commit_message>
<xml_diff>
--- a/공유폴더/REST설계.xlsx
+++ b/공유폴더/REST설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\219\myspringboot\kkfd\공유폴더\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9374871B-D93B-494D-958F-48260EA97365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5129116-F04F-422D-A045-59A2B809C4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77874C4B-F0CC-4F91-8639-CFD8FFB6BE57}"/>
+    <workbookView xWindow="28680" yWindow="1635" windowWidth="29040" windowHeight="15840" xr2:uid="{77874C4B-F0CC-4F91-8639-CFD8FFB6BE57}"/>
   </bookViews>
   <sheets>
     <sheet name="명사" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="170">
   <si>
     <t>회원가입</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -546,10 +546,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>join.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mylist.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -558,18 +554,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/project/{no}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/fundings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/bookmark/{no}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -582,10 +570,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/project/{no}/members</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/funding/{no}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -594,34 +578,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/members</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/creator/projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/creator</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/member/projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/member/{id}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/member/marked-projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/logincheck</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DTO기준</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -630,10 +594,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LoginController</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>메인/목록/상세/마이</t>
   </si>
   <si>
@@ -651,14 +611,6 @@
   </si>
   <si>
     <t>https://developer.cafe24.com/docs/en/api/admin/#api-status-code</t>
-  </si>
-  <si>
-    <t>ProjectListController</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberProjectController</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>/project/{no}/histrory</t>
@@ -674,7 +626,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>info.html /apply.html</t>
+    <t>cmypage.html / register.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>펀딩 참여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크리에이터 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크리에이터 정보수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/logout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/logincheck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/sigup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/funding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -682,11 +670,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cmypage.html / register.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>펀딩 참여</t>
+    <t>MyPageController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>info.html / apply.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/bookmark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member/project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/creator/project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/project/{no}/member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/project/{category}/{state}/{order}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreatorDAO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FundingDAO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProjectDAO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memberDAO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -789,7 +813,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1328,13 +1352,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1515,9 +1548,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1527,12 +1557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1554,6 +1578,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1563,106 +1680,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1677,19 +1734,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2006,11 +2066,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C00F0F0C-FD1C-44BC-9758-3D9C8AFBD163}">
-  <dimension ref="B1:S32"/>
+  <dimension ref="B1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2020,83 +2080,88 @@
     <col min="3" max="3" width="16.125" customWidth="1"/>
     <col min="4" max="4" width="18.125" customWidth="1"/>
     <col min="5" max="5" width="20.25" customWidth="1"/>
-    <col min="6" max="6" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.375" customWidth="1"/>
     <col min="7" max="7" width="11.375" customWidth="1"/>
     <col min="8" max="8" width="25.875" customWidth="1"/>
-    <col min="9" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="10.375" customWidth="1"/>
-    <col min="13" max="13" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.375" customWidth="1"/>
-    <col min="16" max="16" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" customWidth="1"/>
-    <col min="18" max="18" width="17" customWidth="1"/>
-    <col min="19" max="19" width="18.25" customWidth="1"/>
+    <col min="9" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="14.25" customWidth="1"/>
+    <col min="14" max="14" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.375" customWidth="1"/>
+    <col min="17" max="17" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
+    <col min="20" max="20" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I1" t="s">
         <v>48</v>
       </c>
       <c r="L1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="97" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="93" t="s">
+    <row r="2" spans="2:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="81" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="84"/>
-      <c r="G2" s="93" t="s">
+      <c r="F2" s="90"/>
+      <c r="G2" s="88" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95" t="s">
+      <c r="J2" s="97"/>
+      <c r="K2" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95" t="s">
+      <c r="L2" s="97"/>
+      <c r="M2" s="81" t="s">
+        <v>137</v>
+      </c>
+      <c r="N2" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="93" t="s">
+      <c r="O2" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="89" t="s">
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="92" t="s">
         <v>77</v>
       </c>
-      <c r="S2" s="91"/>
-    </row>
-    <row r="3" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="98"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
+      <c r="T2" s="95"/>
+    </row>
+    <row r="3" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="82"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
       <c r="I3" s="46"/>
       <c r="J3" s="44" t="s">
         <v>103</v>
@@ -2105,24 +2170,25 @@
       <c r="L3" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="M3" s="96"/>
-      <c r="N3" s="24" t="s">
+      <c r="M3" s="82"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="P3" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="Q3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="45" t="s">
+      <c r="R3" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="90"/>
-      <c r="S3" s="92"/>
-    </row>
-    <row r="4" spans="2:19" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="62" t="s">
+      <c r="S3" s="93"/>
+      <c r="T3" s="96"/>
+    </row>
+    <row r="4" spans="2:20" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="61" t="s">
         <v>117</v>
       </c>
       <c r="C4" s="39" t="s">
@@ -2143,33 +2209,36 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="11"/>
-    </row>
-    <row r="5" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="76"/>
-      <c r="C5" s="43" t="s">
+      <c r="S4" s="10"/>
+      <c r="T4" s="11"/>
+    </row>
+    <row r="5" spans="2:20" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="83"/>
+      <c r="C5" s="74" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="77" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="43" t="s">
+      <c r="E5" s="110" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="74" t="s">
         <v>116</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -2179,31 +2248,32 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="M5" s="83"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="3"/>
-    </row>
-    <row r="6" spans="2:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="76"/>
-      <c r="C6" s="43" t="s">
+      <c r="S5" s="1"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="2:20" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="83"/>
+      <c r="C6" s="74" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="58" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="43" t="s">
+      <c r="E6" s="108"/>
+      <c r="F6" s="73" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="74" t="s">
         <v>116</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2211,181 +2281,196 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="M6" s="83"/>
+      <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="3"/>
-    </row>
-    <row r="7" spans="2:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="76" t="s">
+      <c r="S6" s="1"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="2:20" s="77" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="41" t="s">
+      <c r="E7" s="108"/>
+      <c r="F7" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="O7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="P7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="64" t="s">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="S7" s="65" t="s">
+      <c r="T7" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="76"/>
-      <c r="C8" s="39" t="s">
+    <row r="8" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="83"/>
+      <c r="C8" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="G8" s="39" t="s">
+      <c r="E8" s="108"/>
+      <c r="F8" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10" t="s">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="O8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="P8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="11"/>
-    </row>
-    <row r="9" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="76"/>
-      <c r="C9" s="43" t="s">
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="83"/>
+      <c r="C9" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="G9" s="43" t="s">
+      <c r="E9" s="109"/>
+      <c r="F9" s="79" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1" t="s">
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="76"/>
-      <c r="C10" s="43" t="s">
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="9"/>
+    </row>
+    <row r="10" spans="2:20" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="83"/>
+      <c r="C10" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="74"/>
-      <c r="F10" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="43" t="s">
+      <c r="E10" s="108" t="s">
+        <v>159</v>
+      </c>
+      <c r="F10" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1" t="s">
+      <c r="H10" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="2:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="76"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="83"/>
       <c r="C11" s="41" t="s">
         <v>55</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="78"/>
-      <c r="F11" s="63" t="s">
-        <v>129</v>
+      <c r="E11" s="108"/>
+      <c r="F11" s="62" t="s">
+        <v>128</v>
       </c>
       <c r="G11" s="41" t="s">
         <v>113</v>
@@ -2395,73 +2480,79 @@
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="L11" s="8"/>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="83"/>
+      <c r="N11" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>42</v>
       </c>
       <c r="P11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
-      <c r="S11" s="9"/>
-    </row>
-    <row r="12" spans="2:19" s="52" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="79" t="s">
+      <c r="S11" s="8"/>
+      <c r="T11" s="9"/>
+    </row>
+    <row r="12" spans="2:20" s="52" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="88" t="s">
-        <v>156</v>
-      </c>
+      <c r="E12" s="108"/>
       <c r="F12" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="G12" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68" t="s">
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="L12" s="65"/>
+      <c r="M12" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="N12" s="68" t="s">
+      <c r="O12" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="69"/>
-    </row>
-    <row r="13" spans="2:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="80"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="66"/>
+    </row>
+    <row r="13" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="85"/>
       <c r="C13" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="87"/>
-      <c r="F13" s="63" t="s">
-        <v>144</v>
+        <v>134</v>
+      </c>
+      <c r="E13" s="109"/>
+      <c r="F13" s="62" t="s">
+        <v>161</v>
       </c>
       <c r="G13" s="41" t="s">
         <v>113</v>
@@ -2471,564 +2562,657 @@
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="K13" s="8" t="s">
+        <v>168</v>
+      </c>
       <c r="L13" s="8"/>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="85"/>
+      <c r="N13" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="O13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
-    </row>
-    <row r="14" spans="2:19" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="76" t="s">
-        <v>147</v>
+      <c r="S13" s="8"/>
+      <c r="T13" s="9"/>
+    </row>
+    <row r="14" spans="2:20" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="83" t="s">
+        <v>138</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="103" t="s">
         <v>119</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G14" s="40" t="s">
         <v>114</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>166</v>
+      </c>
       <c r="L14" s="6"/>
-      <c r="M14" s="6" t="s">
-        <v>107</v>
+      <c r="M14" s="83" t="s">
+        <v>138</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" s="6"/>
+        <v>108</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
-      <c r="S14" s="7"/>
-    </row>
-    <row r="15" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="76"/>
-      <c r="C15" s="43" t="s">
+      <c r="S14" s="6"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="83"/>
+      <c r="C15" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="103"/>
+      <c r="F15" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="83"/>
+      <c r="C16" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="86"/>
-      <c r="F15" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="G15" s="43" t="s">
+      <c r="D16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="104"/>
+      <c r="F16" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1" t="s">
+      <c r="H16" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="3"/>
-    </row>
-    <row r="16" spans="2:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="79" t="s">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C17" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="87"/>
-      <c r="F16" s="63" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" s="41" t="s">
+      <c r="E17" s="105"/>
+      <c r="F17" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8" t="s">
+      <c r="H17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="O17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="9"/>
-    </row>
-    <row r="17" spans="2:19" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
-      <c r="C17" s="39" t="s">
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="9"/>
+    </row>
+    <row r="18" spans="2:20" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="86"/>
+      <c r="C18" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="88" t="s">
+      <c r="E18" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="L18" s="10"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="11"/>
+    </row>
+    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="86"/>
+      <c r="C19" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="104"/>
+      <c r="F19" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="86"/>
+      <c r="C20" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="105"/>
+      <c r="F20" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L20" s="8"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="9"/>
+    </row>
+    <row r="21" spans="2:20" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="86"/>
+      <c r="C21" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="68" t="s">
         <v>155</v>
       </c>
-      <c r="F17" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="N17" s="10" t="s">
+      <c r="G21" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" s="54"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="O21" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="55"/>
+    </row>
+    <row r="22" spans="2:20" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="85"/>
+      <c r="C22" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="102" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="2:20" s="47" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="107"/>
+      <c r="F23" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L23" s="8"/>
+      <c r="M23" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="O23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="11"/>
-    </row>
-    <row r="18" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="82"/>
-      <c r="C18" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="58" t="s">
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="9"/>
+    </row>
+    <row r="24" spans="2:20" s="47" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="83"/>
+      <c r="C24" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" s="101" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L24" s="6"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="83"/>
+      <c r="C25" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="H18" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="3"/>
-    </row>
-    <row r="19" spans="2:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="82"/>
-      <c r="C19" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="87"/>
-      <c r="F19" s="63" t="s">
-        <v>157</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="H19" s="66" t="s">
-        <v>159</v>
-      </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="9"/>
-    </row>
-    <row r="20" spans="2:19" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="82"/>
-      <c r="C20" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="F20" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="N20" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="O20" s="54"/>
-      <c r="P20" s="54"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="55"/>
-    </row>
-    <row r="21" spans="2:19" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="80"/>
-      <c r="C21" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="74" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="56" t="s">
-        <v>131</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="7"/>
-    </row>
-    <row r="22" spans="2:19" s="47" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="78"/>
-      <c r="F22" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="H22" s="8" t="s">
+      <c r="E25" s="102"/>
+      <c r="F25" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="G25" s="43"/>
+      <c r="H25" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="9"/>
-    </row>
-    <row r="23" spans="2:19" s="47" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="76"/>
-      <c r="C23" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="7"/>
-    </row>
-    <row r="24" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="76"/>
-      <c r="C24" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" s="74"/>
-      <c r="F24" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="3"/>
-    </row>
-    <row r="25" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="76"/>
-      <c r="C25" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="E25" s="75"/>
-      <c r="F25" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="G25" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+      <c r="K25" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="M25" s="83"/>
       <c r="N25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O25" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="3"/>
-    </row>
-    <row r="26" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="76" t="s">
-        <v>62</v>
-      </c>
+      <c r="S25" s="1"/>
+      <c r="T25" s="3"/>
+    </row>
+    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="83"/>
       <c r="C26" s="43" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="77" t="s">
-        <v>121</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E26" s="103"/>
       <c r="F26" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="G26" s="43"/>
+        <v>156</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>115</v>
+      </c>
       <c r="H26" s="1" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="1" t="s">
+      <c r="M26" s="83"/>
+      <c r="N26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="3"/>
-    </row>
-    <row r="27" spans="2:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="81"/>
-      <c r="C27" s="42" t="s">
+      <c r="S26" s="1"/>
+      <c r="T26" s="3"/>
+    </row>
+    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" s="43"/>
+      <c r="H27" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="87"/>
+      <c r="C28" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D28" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4" t="s">
+      <c r="E28" s="100"/>
+      <c r="F28" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="42"/>
+      <c r="H28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="O28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="5"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="C29" s="13"/>
-      <c r="D29" t="s">
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="5"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C30" s="13"/>
+      <c r="D30" t="s">
         <v>60</v>
       </c>
-      <c r="F29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
-        <v>154</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="35">
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E5:E9"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="M17:M22"/>
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="M27:M28"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="E22:E23"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="M14:M16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3042,7 +3226,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22:B23"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3082,62 +3266,62 @@
       </c>
     </row>
     <row r="2" spans="2:28" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="114" t="s">
+      <c r="E2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="114" t="s">
+      <c r="H2" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="112" t="s">
+      <c r="J2" s="120" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="113"/>
-      <c r="L2" s="112" t="s">
+      <c r="K2" s="121"/>
+      <c r="L2" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="M2" s="113"/>
-      <c r="N2" s="110" t="s">
+      <c r="M2" s="121"/>
+      <c r="N2" s="118" t="s">
         <v>74</v>
       </c>
       <c r="O2" s="27"/>
-      <c r="P2" s="93" t="s">
+      <c r="P2" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="89" t="s">
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="92" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="91"/>
+      <c r="U2" s="95"/>
     </row>
     <row r="3" spans="2:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="118"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
       <c r="J3" s="46"/>
       <c r="K3" s="29" t="s">
         <v>103</v>
@@ -3146,7 +3330,7 @@
       <c r="M3" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="N3" s="111"/>
+      <c r="N3" s="119"/>
       <c r="O3" s="28"/>
       <c r="P3" s="24" t="s">
         <v>65</v>
@@ -3160,8 +3344,8 @@
       <c r="S3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="90"/>
-      <c r="U3" s="92"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="96"/>
     </row>
     <row r="4" spans="2:28" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
@@ -3202,7 +3386,7 @@
       <c r="U4" s="23"/>
     </row>
     <row r="5" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="111" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -3214,7 +3398,7 @@
       <c r="E5" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="112" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -3244,7 +3428,7 @@
       <c r="U5" s="11"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B6" s="82"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
@@ -3254,7 +3438,7 @@
       <c r="E6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="116"/>
+      <c r="F6" s="113"/>
       <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
@@ -3280,7 +3464,7 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B7" s="82"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
@@ -3290,7 +3474,7 @@
       <c r="E7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="116"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="1" t="s">
         <v>16</v>
       </c>
@@ -3322,7 +3506,7 @@
       </c>
     </row>
     <row r="8" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="82"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="1" t="s">
         <v>53</v>
       </c>
@@ -3332,7 +3516,7 @@
       <c r="E8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="116"/>
+      <c r="F8" s="113"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
@@ -3358,7 +3542,7 @@
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
@@ -3368,7 +3552,7 @@
       <c r="E9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="116"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
@@ -3394,7 +3578,7 @@
       <c r="U9" s="3"/>
     </row>
     <row r="10" spans="2:28" ht="33" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="1" t="s">
         <v>53</v>
       </c>
@@ -3404,7 +3588,7 @@
       <c r="E10" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F10" s="116"/>
+      <c r="F10" s="113"/>
       <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
@@ -3433,7 +3617,7 @@
       </c>
     </row>
     <row r="11" spans="2:28" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="82"/>
+      <c r="B11" s="86"/>
       <c r="C11" s="1" t="s">
         <v>55</v>
       </c>
@@ -3443,7 +3627,7 @@
       <c r="E11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="116"/>
+      <c r="F11" s="113"/>
       <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
@@ -3475,7 +3659,7 @@
       <c r="U11" s="3"/>
     </row>
     <row r="12" spans="2:28" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="111" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -3487,7 +3671,7 @@
       <c r="E12" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="107" t="s">
+      <c r="F12" s="127" t="s">
         <v>79</v>
       </c>
       <c r="G12" s="10" t="s">
@@ -3517,7 +3701,7 @@
       <c r="U12" s="11"/>
     </row>
     <row r="13" spans="2:28" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="101"/>
+      <c r="B13" s="122"/>
       <c r="C13" s="8" t="s">
         <v>55</v>
       </c>
@@ -3555,7 +3739,7 @@
       <c r="U13" s="9"/>
     </row>
     <row r="14" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="111" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -3567,7 +3751,7 @@
       <c r="E14" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="107" t="s">
+      <c r="F14" s="127" t="s">
         <v>57</v>
       </c>
       <c r="G14" s="10" t="s">
@@ -3603,7 +3787,7 @@
       </c>
     </row>
     <row r="15" spans="2:28" ht="33" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
+      <c r="B15" s="86"/>
       <c r="C15" s="1" t="s">
         <v>53</v>
       </c>
@@ -3641,7 +3825,7 @@
       <c r="U15" s="7"/>
     </row>
     <row r="16" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="1" t="s">
         <v>53</v>
       </c>
@@ -3679,7 +3863,7 @@
       <c r="U16" s="7"/>
     </row>
     <row r="17" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="1" t="s">
         <v>53</v>
       </c>
@@ -3717,7 +3901,7 @@
       <c r="U17" s="3"/>
     </row>
     <row r="18" spans="2:21" s="52" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="82"/>
+      <c r="B18" s="86"/>
       <c r="C18" s="49" t="s">
         <v>53</v>
       </c>
@@ -3755,7 +3939,7 @@
       <c r="U18" s="51"/>
     </row>
     <row r="19" spans="2:21" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="82"/>
+      <c r="B19" s="86"/>
       <c r="C19" s="6" t="s">
         <v>54</v>
       </c>
@@ -3795,7 +3979,7 @@
       <c r="U19" s="7"/>
     </row>
     <row r="20" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="82"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
@@ -3833,7 +4017,7 @@
       <c r="U20" s="3"/>
     </row>
     <row r="21" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="101"/>
+      <c r="B21" s="122"/>
       <c r="C21" s="8" t="s">
         <v>55</v>
       </c>
@@ -3871,7 +4055,7 @@
       <c r="U21" s="9"/>
     </row>
     <row r="22" spans="2:21" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="111" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -3883,7 +4067,7 @@
       <c r="E22" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F22" s="103" t="s">
+      <c r="F22" s="112" t="s">
         <v>58</v>
       </c>
       <c r="G22" s="10" t="s">
@@ -3913,7 +4097,7 @@
       <c r="U22" s="11"/>
     </row>
     <row r="23" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="101"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="8" t="s">
         <v>55</v>
       </c>
@@ -3923,7 +4107,7 @@
       <c r="E23" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="104"/>
+      <c r="F23" s="124"/>
       <c r="G23" s="8" t="s">
         <v>36</v>
       </c>
@@ -3951,7 +4135,7 @@
       <c r="U23" s="9"/>
     </row>
     <row r="24" spans="2:21" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="111" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -3961,7 +4145,7 @@
         <v>13</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="105" t="s">
+      <c r="F24" s="125" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="6" t="s">
@@ -3987,7 +4171,7 @@
       <c r="U24" s="7"/>
     </row>
     <row r="25" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="102"/>
+      <c r="B25" s="123"/>
       <c r="C25" s="4" t="s">
         <v>56</v>
       </c>
@@ -3995,7 +4179,7 @@
         <v>14</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="106"/>
+      <c r="F25" s="126"/>
       <c r="G25" s="4" t="s">
         <v>27</v>
       </c>
@@ -4050,13 +4234,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="F5:F11"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="P2:S2"/>
@@ -4066,15 +4252,13 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="F5:F11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#10공유폴더 수정 mybatis-config.xml 수정
</commit_message>
<xml_diff>
--- a/공유폴더/REST설계.xlsx
+++ b/공유폴더/REST설계.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\219\myspringboot\kkfd\공유폴더\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F7D9CE-DED0-4161-BA67-852FB535AF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A753FBA-29C7-48E5-A0B4-D9010776D31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1635" windowWidth="29040" windowHeight="15840" xr2:uid="{77874C4B-F0CC-4F91-8639-CFD8FFB6BE57}"/>
   </bookViews>
@@ -682,10 +682,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/project/{no}/member</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CreatorDAO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -778,6 +774,10 @@
   </si>
   <si>
     <t>ProjectMainDAO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/project/{projNo}/fundings</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1710,6 +1710,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1788,48 +1797,51 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1847,18 +1859,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2176,9 +2176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C00F0F0C-FD1C-44BC-9758-3D9C8AFBD163}">
   <dimension ref="B1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2221,76 +2221,76 @@
       </c>
     </row>
     <row r="2" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="95" t="s">
+      <c r="E2" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="95"/>
-      <c r="G2" s="93" t="s">
+      <c r="F2" s="98"/>
+      <c r="G2" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="124" t="s">
+      <c r="I2" s="120" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="134"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="111" t="s">
+      <c r="J2" s="121"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="114" t="s">
         <v>106</v>
       </c>
-      <c r="M2" s="111"/>
-      <c r="N2" s="122" t="s">
+      <c r="M2" s="114"/>
+      <c r="N2" s="115" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="91" t="s">
+      <c r="O2" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="P2" s="93" t="s">
+      <c r="P2" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="106" t="s">
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="109"/>
+      <c r="U2" s="112"/>
     </row>
     <row r="3" spans="2:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="92"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
       <c r="I3" s="80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J3" s="44" t="s">
         <v>103</v>
       </c>
       <c r="K3" s="80" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M3" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="N3" s="123"/>
-      <c r="O3" s="92"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="95"/>
       <c r="P3" s="24" t="s">
         <v>65</v>
       </c>
@@ -2303,8 +2303,8 @@
       <c r="S3" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="107"/>
-      <c r="U3" s="110"/>
+      <c r="T3" s="110"/>
+      <c r="U3" s="113"/>
     </row>
     <row r="4" spans="2:21" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="61" t="s">
@@ -2328,7 +2328,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10" t="s">
@@ -2347,14 +2347,14 @@
       <c r="U4" s="11"/>
     </row>
     <row r="5" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="86"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="73" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="119" t="s">
         <v>118</v>
       </c>
       <c r="F5" s="72" t="s">
@@ -2372,7 +2372,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="86"/>
+      <c r="O5" s="89"/>
       <c r="P5" s="1" t="s">
         <v>43</v>
       </c>
@@ -2385,14 +2385,14 @@
       <c r="U5" s="3"/>
     </row>
     <row r="6" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="86"/>
+      <c r="B6" s="89"/>
       <c r="C6" s="73" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="112"/>
+      <c r="E6" s="117"/>
       <c r="F6" s="72" t="s">
         <v>152</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="86"/>
+      <c r="O6" s="89"/>
       <c r="P6" s="1" t="s">
         <v>43</v>
       </c>
@@ -2421,7 +2421,7 @@
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="2:21" s="76" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="89" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="73" t="s">
@@ -2430,7 +2430,7 @@
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="112"/>
+      <c r="E7" s="117"/>
       <c r="F7" s="72" t="s">
         <v>156</v>
       </c>
@@ -2444,13 +2444,13 @@
       <c r="J7" s="1"/>
       <c r="K7" s="6"/>
       <c r="L7" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O7" s="86" t="s">
+      <c r="O7" s="89" t="s">
         <v>3</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -2469,14 +2469,14 @@
       </c>
     </row>
     <row r="8" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="86"/>
+      <c r="B8" s="89"/>
       <c r="C8" s="75" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="112"/>
+      <c r="E8" s="117"/>
       <c r="F8" s="71" t="s">
         <v>153</v>
       </c>
@@ -2490,13 +2490,13 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="O8" s="86"/>
+      <c r="O8" s="89"/>
       <c r="P8" s="6" t="s">
         <v>41</v>
       </c>
@@ -2509,14 +2509,14 @@
       <c r="U8" s="7"/>
     </row>
     <row r="9" spans="2:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="86"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="74" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="113"/>
+      <c r="E9" s="118"/>
       <c r="F9" s="78" t="s">
         <v>136</v>
       </c>
@@ -2530,13 +2530,13 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="82" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="O9" s="86"/>
+      <c r="O9" s="89"/>
       <c r="P9" s="8" t="s">
         <v>39</v>
       </c>
@@ -2549,14 +2549,14 @@
       <c r="U9" s="9"/>
     </row>
     <row r="10" spans="2:21" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="86"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="75" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="112" t="s">
+      <c r="E10" s="117" t="s">
         <v>158</v>
       </c>
       <c r="F10" s="71" t="s">
@@ -2572,13 +2572,13 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="O10" s="86"/>
+      <c r="O10" s="89"/>
       <c r="P10" s="6" t="s">
         <v>39</v>
       </c>
@@ -2589,14 +2589,14 @@
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="2:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="86"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="41" t="s">
         <v>55</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="112"/>
+      <c r="E11" s="117"/>
       <c r="F11" s="62" t="s">
         <v>128</v>
       </c>
@@ -2610,13 +2610,13 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="82" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="O11" s="86"/>
+      <c r="O11" s="89"/>
       <c r="P11" s="8" t="s">
         <v>42</v>
       </c>
@@ -2631,7 +2631,7 @@
       <c r="U11" s="9"/>
     </row>
     <row r="12" spans="2:21" s="52" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="90" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="64" t="s">
@@ -2640,7 +2640,7 @@
       <c r="D12" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="112"/>
+      <c r="E12" s="117"/>
       <c r="F12" s="57" t="s">
         <v>161</v>
       </c>
@@ -2654,13 +2654,13 @@
       <c r="J12" s="65"/>
       <c r="K12" s="65"/>
       <c r="L12" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M12" s="65"/>
       <c r="N12" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="O12" s="87" t="s">
+      <c r="O12" s="90" t="s">
         <v>4</v>
       </c>
       <c r="P12" s="65" t="s">
@@ -2673,14 +2673,14 @@
       <c r="U12" s="66"/>
     </row>
     <row r="13" spans="2:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="88"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E13" s="113"/>
+      <c r="E13" s="118"/>
       <c r="F13" s="62" t="s">
         <v>160</v>
       </c>
@@ -2694,13 +2694,13 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="82" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="O13" s="88"/>
+      <c r="O13" s="91"/>
       <c r="P13" s="8" t="s">
         <v>39</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="U13" s="9"/>
     </row>
     <row r="14" spans="2:21" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="89" t="s">
         <v>138</v>
       </c>
       <c r="C14" s="40" t="s">
@@ -2720,7 +2720,7 @@
       <c r="D14" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="101" t="s">
+      <c r="E14" s="104" t="s">
         <v>119</v>
       </c>
       <c r="F14" s="56" t="s">
@@ -2730,19 +2730,19 @@
         <v>114</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="83" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="O14" s="86" t="s">
+      <c r="O14" s="89" t="s">
         <v>138</v>
       </c>
       <c r="P14" s="6" t="s">
@@ -2755,14 +2755,14 @@
       <c r="U14" s="7"/>
     </row>
     <row r="15" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="86"/>
+      <c r="B15" s="89"/>
       <c r="C15" s="70" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="101"/>
+      <c r="E15" s="104"/>
       <c r="F15" s="69" t="s">
         <v>135</v>
       </c>
@@ -2770,19 +2770,19 @@
         <v>114</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="83" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="O15" s="86"/>
+      <c r="O15" s="89"/>
       <c r="P15" s="6" t="s">
         <v>39</v>
       </c>
@@ -2793,14 +2793,14 @@
       <c r="U15" s="7"/>
     </row>
     <row r="16" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="86"/>
+      <c r="B16" s="89"/>
       <c r="C16" s="43" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E16" s="102"/>
+      <c r="E16" s="105"/>
       <c r="F16" s="58" t="s">
         <v>135</v>
       </c>
@@ -2808,19 +2808,19 @@
         <v>114</v>
       </c>
       <c r="H16" s="59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O16" s="86"/>
+      <c r="O16" s="89"/>
       <c r="P16" s="1" t="s">
         <v>42</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="U16" s="3"/>
     </row>
     <row r="17" spans="2:21" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="90" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="41" t="s">
@@ -2840,9 +2840,9 @@
       <c r="D17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="103"/>
+      <c r="E17" s="106"/>
       <c r="F17" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G17" s="41" t="s">
         <v>114</v>
@@ -2851,31 +2851,31 @@
         <v>127</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J17" s="135" t="s">
-        <v>179</v>
-      </c>
-      <c r="K17" s="135" t="s">
-        <v>176</v>
+        <v>167</v>
+      </c>
+      <c r="J17" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="K17" s="88" t="s">
+        <v>175</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>165</v>
-      </c>
-      <c r="M17" s="135" t="s">
-        <v>175</v>
+        <v>164</v>
+      </c>
+      <c r="M17" s="88" t="s">
+        <v>174</v>
       </c>
       <c r="N17" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="O17" s="87" t="s">
+      <c r="O17" s="90" t="s">
         <v>4</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Q17" s="135" t="s">
-        <v>175</v>
+      <c r="Q17" s="88" t="s">
+        <v>174</v>
       </c>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
@@ -2883,17 +2883,17 @@
       <c r="U17" s="9"/>
     </row>
     <row r="18" spans="2:21" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="89"/>
+      <c r="B18" s="92"/>
       <c r="C18" s="39" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="104" t="s">
+      <c r="E18" s="107" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="133" t="s">
+      <c r="F18" s="87" t="s">
         <v>154</v>
       </c>
       <c r="G18" s="39" t="s">
@@ -2903,24 +2903,24 @@
         <v>91</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K18" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="L18" s="81" t="s">
+        <v>164</v>
+      </c>
+      <c r="M18" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="L18" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="N18" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="O18" s="89"/>
+      <c r="O18" s="92"/>
       <c r="P18" s="10" t="s">
         <v>39</v>
       </c>
@@ -2931,14 +2931,14 @@
       <c r="U18" s="11"/>
     </row>
     <row r="19" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="89"/>
+      <c r="B19" s="92"/>
       <c r="C19" s="43" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="102"/>
+      <c r="E19" s="105"/>
       <c r="F19" s="58" t="s">
         <v>129</v>
       </c>
@@ -2949,29 +2949,29 @@
         <v>159</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L19" s="85" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O19" s="89"/>
+      <c r="O19" s="92"/>
       <c r="P19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -2979,14 +2979,14 @@
       <c r="U19" s="3"/>
     </row>
     <row r="20" spans="2:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="89"/>
+      <c r="B20" s="92"/>
       <c r="C20" s="41" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="103"/>
+      <c r="E20" s="106"/>
       <c r="F20" s="62" t="s">
         <v>145</v>
       </c>
@@ -2997,20 +2997,20 @@
         <v>147</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L20" s="82" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="O20" s="89"/>
+      <c r="O20" s="92"/>
       <c r="P20" s="8" t="s">
         <v>39</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="U20" s="9"/>
     </row>
     <row r="21" spans="2:21" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="89"/>
+      <c r="B21" s="92"/>
       <c r="C21" s="53" t="s">
         <v>54</v>
       </c>
@@ -3031,26 +3031,26 @@
       <c r="E21" s="68" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="132" t="s">
+      <c r="F21" s="86" t="s">
         <v>154</v>
       </c>
       <c r="G21" s="53" t="s">
         <v>116</v>
       </c>
       <c r="H21" s="68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I21" s="54"/>
       <c r="J21" s="54"/>
       <c r="K21" s="54"/>
       <c r="L21" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M21" s="54"/>
       <c r="N21" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="O21" s="89"/>
+      <c r="O21" s="92"/>
       <c r="P21" s="54" t="s">
         <v>41</v>
       </c>
@@ -3061,15 +3061,15 @@
       <c r="U21" s="55"/>
     </row>
     <row r="22" spans="2:21" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="88"/>
+      <c r="B22" s="91"/>
       <c r="C22" s="40" t="s">
         <v>55</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="100" t="s">
-        <v>182</v>
+      <c r="E22" s="103" t="s">
+        <v>181</v>
       </c>
       <c r="F22" s="56" t="s">
         <v>129</v>
@@ -3081,18 +3081,18 @@
         <v>127</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="83" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="O22" s="88"/>
+      <c r="O22" s="91"/>
       <c r="P22" s="6" t="s">
         <v>42</v>
       </c>
@@ -3103,7 +3103,7 @@
       <c r="U22" s="7"/>
     </row>
     <row r="23" spans="2:21" s="47" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="89" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="41" t="s">
@@ -3112,9 +3112,9 @@
       <c r="D23" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="105"/>
+      <c r="E23" s="108"/>
       <c r="F23" s="62" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="G23" s="41" t="s">
         <v>114</v>
@@ -3123,18 +3123,18 @@
         <v>123</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="O23" s="86" t="s">
+      <c r="O23" s="89" t="s">
         <v>7</v>
       </c>
       <c r="P23" s="8" t="s">
@@ -3147,14 +3147,14 @@
       <c r="U23" s="9"/>
     </row>
     <row r="24" spans="2:21" s="47" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="86"/>
+      <c r="B24" s="89"/>
       <c r="C24" s="40" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E24" s="99" t="s">
+      <c r="E24" s="102" t="s">
         <v>126</v>
       </c>
       <c r="F24" s="56" t="s">
@@ -3170,13 +3170,13 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M24" s="6"/>
       <c r="N24" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="O24" s="86"/>
+      <c r="O24" s="89"/>
       <c r="P24" s="6" t="s">
         <v>42</v>
       </c>
@@ -3187,14 +3187,14 @@
       <c r="U24" s="7"/>
     </row>
     <row r="25" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="86"/>
+      <c r="B25" s="89"/>
       <c r="C25" s="43" t="s">
         <v>55</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="100"/>
+      <c r="E25" s="103"/>
       <c r="F25" s="58" t="s">
         <v>155</v>
       </c>
@@ -3206,13 +3206,13 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O25" s="86"/>
+      <c r="O25" s="89"/>
       <c r="P25" s="1" t="s">
         <v>42</v>
       </c>
@@ -3223,14 +3223,14 @@
       <c r="U25" s="3"/>
     </row>
     <row r="26" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="86"/>
+      <c r="B26" s="89"/>
       <c r="C26" s="43" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="E26" s="101"/>
+      <c r="E26" s="104"/>
       <c r="F26" s="58" t="s">
         <v>155</v>
       </c>
@@ -3244,13 +3244,13 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O26" s="86"/>
+      <c r="O26" s="89"/>
       <c r="P26" s="1" t="s">
         <v>41</v>
       </c>
@@ -3261,7 +3261,7 @@
       <c r="U26" s="3"/>
     </row>
     <row r="27" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="86" t="s">
+      <c r="B27" s="89" t="s">
         <v>62</v>
       </c>
       <c r="C27" s="43" t="s">
@@ -3270,7 +3270,7 @@
       <c r="D27" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="97" t="s">
+      <c r="E27" s="100" t="s">
         <v>121</v>
       </c>
       <c r="F27" s="58" t="s">
@@ -3288,7 +3288,7 @@
       <c r="N27" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O27" s="86" t="s">
+      <c r="O27" s="89" t="s">
         <v>62</v>
       </c>
       <c r="P27" s="1" t="s">
@@ -3301,14 +3301,14 @@
       <c r="U27" s="3"/>
     </row>
     <row r="28" spans="2:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="90"/>
+      <c r="B28" s="93"/>
       <c r="C28" s="42" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="98"/>
+      <c r="E28" s="101"/>
       <c r="F28" s="60" t="s">
         <v>130</v>
       </c>
@@ -3324,7 +3324,7 @@
       <c r="N28" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="O28" s="90"/>
+      <c r="O28" s="93"/>
       <c r="P28" s="4" t="s">
         <v>84</v>
       </c>
@@ -3448,62 +3448,62 @@
       </c>
     </row>
     <row r="2" spans="2:28" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="120" t="s">
+      <c r="E2" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="95" t="s">
+      <c r="F2" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="120" t="s">
+      <c r="H2" s="128" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="120" t="s">
+      <c r="I2" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="124" t="s">
+      <c r="J2" s="120" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="125"/>
-      <c r="L2" s="124" t="s">
+      <c r="K2" s="122"/>
+      <c r="L2" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="M2" s="125"/>
-      <c r="N2" s="122" t="s">
+      <c r="M2" s="122"/>
+      <c r="N2" s="115" t="s">
         <v>74</v>
       </c>
       <c r="O2" s="27"/>
-      <c r="P2" s="93" t="s">
+      <c r="P2" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="106" t="s">
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="109"/>
+      <c r="U2" s="112"/>
     </row>
     <row r="3" spans="2:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="119"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
       <c r="J3" s="46"/>
       <c r="K3" s="29" t="s">
         <v>103</v>
@@ -3512,7 +3512,7 @@
       <c r="M3" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="N3" s="123"/>
+      <c r="N3" s="116"/>
       <c r="O3" s="28"/>
       <c r="P3" s="24" t="s">
         <v>65</v>
@@ -3526,8 +3526,8 @@
       <c r="S3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="107"/>
-      <c r="U3" s="110"/>
+      <c r="T3" s="110"/>
+      <c r="U3" s="113"/>
     </row>
     <row r="4" spans="2:28" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
@@ -3568,7 +3568,7 @@
       <c r="U4" s="23"/>
     </row>
     <row r="5" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="123" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -3580,7 +3580,7 @@
       <c r="E5" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="116" t="s">
+      <c r="F5" s="124" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -3610,7 +3610,7 @@
       <c r="U5" s="11"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B6" s="89"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
@@ -3620,7 +3620,7 @@
       <c r="E6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="117"/>
+      <c r="F6" s="125"/>
       <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
@@ -3646,7 +3646,7 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B7" s="89"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
@@ -3656,7 +3656,7 @@
       <c r="E7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="117"/>
+      <c r="F7" s="125"/>
       <c r="G7" s="1" t="s">
         <v>16</v>
       </c>
@@ -3688,7 +3688,7 @@
       </c>
     </row>
     <row r="8" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="89"/>
+      <c r="B8" s="92"/>
       <c r="C8" s="1" t="s">
         <v>53</v>
       </c>
@@ -3698,7 +3698,7 @@
       <c r="E8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="117"/>
+      <c r="F8" s="125"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
@@ -3724,7 +3724,7 @@
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="89"/>
+      <c r="B9" s="92"/>
       <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="E9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="117"/>
+      <c r="F9" s="125"/>
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="U9" s="3"/>
     </row>
     <row r="10" spans="2:28" ht="33" x14ac:dyDescent="0.3">
-      <c r="B10" s="89"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="1" t="s">
         <v>53</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="E10" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F10" s="117"/>
+      <c r="F10" s="125"/>
       <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
@@ -3799,7 +3799,7 @@
       </c>
     </row>
     <row r="11" spans="2:28" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="89"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="1" t="s">
         <v>55</v>
       </c>
@@ -3809,7 +3809,7 @@
       <c r="E11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="117"/>
+      <c r="F11" s="125"/>
       <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
@@ -3841,7 +3841,7 @@
       <c r="U11" s="3"/>
     </row>
     <row r="12" spans="2:28" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="115" t="s">
+      <c r="B12" s="123" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -3853,7 +3853,7 @@
       <c r="E12" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="131" t="s">
+      <c r="F12" s="135" t="s">
         <v>79</v>
       </c>
       <c r="G12" s="10" t="s">
@@ -3883,7 +3883,7 @@
       <c r="U12" s="11"/>
     </row>
     <row r="13" spans="2:28" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="126"/>
+      <c r="B13" s="130"/>
       <c r="C13" s="8" t="s">
         <v>55</v>
       </c>
@@ -3893,7 +3893,7 @@
       <c r="E13" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="113"/>
+      <c r="F13" s="118"/>
       <c r="G13" s="8" t="s">
         <v>81</v>
       </c>
@@ -3921,7 +3921,7 @@
       <c r="U13" s="9"/>
     </row>
     <row r="14" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="123" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -3933,7 +3933,7 @@
       <c r="E14" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="131" t="s">
+      <c r="F14" s="135" t="s">
         <v>57</v>
       </c>
       <c r="G14" s="10" t="s">
@@ -3969,7 +3969,7 @@
       </c>
     </row>
     <row r="15" spans="2:28" ht="33" x14ac:dyDescent="0.3">
-      <c r="B15" s="89"/>
+      <c r="B15" s="92"/>
       <c r="C15" s="1" t="s">
         <v>53</v>
       </c>
@@ -3979,7 +3979,7 @@
       <c r="E15" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="112"/>
+      <c r="F15" s="117"/>
       <c r="G15" s="1" t="s">
         <v>27</v>
       </c>
@@ -4007,7 +4007,7 @@
       <c r="U15" s="7"/>
     </row>
     <row r="16" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="89"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="1" t="s">
         <v>53</v>
       </c>
@@ -4017,7 +4017,7 @@
       <c r="E16" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="112"/>
+      <c r="F16" s="117"/>
       <c r="G16" s="1" t="s">
         <v>28</v>
       </c>
@@ -4045,7 +4045,7 @@
       <c r="U16" s="7"/>
     </row>
     <row r="17" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="89"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="1" t="s">
         <v>53</v>
       </c>
@@ -4055,7 +4055,7 @@
       <c r="E17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="112"/>
+      <c r="F17" s="117"/>
       <c r="G17" s="1" t="s">
         <v>32</v>
       </c>
@@ -4083,7 +4083,7 @@
       <c r="U17" s="3"/>
     </row>
     <row r="18" spans="2:21" s="52" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="89"/>
+      <c r="B18" s="92"/>
       <c r="C18" s="49" t="s">
         <v>53</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="E18" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="113"/>
+      <c r="F18" s="118"/>
       <c r="G18" s="49" t="s">
         <v>37</v>
       </c>
@@ -4121,7 +4121,7 @@
       <c r="U18" s="51"/>
     </row>
     <row r="19" spans="2:21" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="89"/>
+      <c r="B19" s="92"/>
       <c r="C19" s="6" t="s">
         <v>54</v>
       </c>
@@ -4131,7 +4131,7 @@
       <c r="E19" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="112" t="s">
+      <c r="F19" s="117" t="s">
         <v>112</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -4161,7 +4161,7 @@
       <c r="U19" s="7"/>
     </row>
     <row r="20" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="89"/>
+      <c r="B20" s="92"/>
       <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
@@ -4171,7 +4171,7 @@
       <c r="E20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="112"/>
+      <c r="F20" s="117"/>
       <c r="G20" s="1" t="s">
         <v>30</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="U20" s="3"/>
     </row>
     <row r="21" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="126"/>
+      <c r="B21" s="130"/>
       <c r="C21" s="8" t="s">
         <v>55</v>
       </c>
@@ -4209,7 +4209,7 @@
       <c r="E21" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="113"/>
+      <c r="F21" s="118"/>
       <c r="G21" s="8" t="s">
         <v>27</v>
       </c>
@@ -4237,7 +4237,7 @@
       <c r="U21" s="9"/>
     </row>
     <row r="22" spans="2:21" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="115" t="s">
+      <c r="B22" s="123" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -4249,7 +4249,7 @@
       <c r="E22" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F22" s="116" t="s">
+      <c r="F22" s="124" t="s">
         <v>58</v>
       </c>
       <c r="G22" s="10" t="s">
@@ -4279,7 +4279,7 @@
       <c r="U22" s="11"/>
     </row>
     <row r="23" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="126"/>
+      <c r="B23" s="130"/>
       <c r="C23" s="8" t="s">
         <v>55</v>
       </c>
@@ -4289,7 +4289,7 @@
       <c r="E23" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="128"/>
+      <c r="F23" s="132"/>
       <c r="G23" s="8" t="s">
         <v>36</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="U23" s="9"/>
     </row>
     <row r="24" spans="2:21" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="115" t="s">
+      <c r="B24" s="123" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -4327,7 +4327,7 @@
         <v>13</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="129" t="s">
+      <c r="F24" s="133" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="6" t="s">
@@ -4353,7 +4353,7 @@
       <c r="U24" s="7"/>
     </row>
     <row r="25" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="127"/>
+      <c r="B25" s="131"/>
       <c r="C25" s="4" t="s">
         <v>56</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>14</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="130"/>
+      <c r="F25" s="134"/>
       <c r="G25" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>